<commit_message>
Creación del modelo Medico, para recibir document del Médico desde el formato de excel y admisionarlo por actividad
</commit_message>
<xml_diff>
--- a/media/forma_carga_actividad_plantilla.xlsx
+++ b/media/forma_carga_actividad_plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sersocial-my.sharepoint.com/personal/jrueda_sersocial_org/Documents/Documentos/Proyectos SerSocial/zagilad/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sersocial-my.sharepoint.com/personal/jrueda_sersocial_org/Documents/Documentos/Proyectos SerSocial/zagilad/zagilad/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F6564E-16B6-4BF1-8E2E-8F7780CB7DA5}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E1CD3DF-AC93-4B73-8F27-9D1F79EA47FA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tipo de Identificación del Usuario</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>CIE10</t>
+  </si>
+  <si>
+    <t>Identificación médico</t>
   </si>
 </sst>
 </file>
@@ -584,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,9 +605,10 @@
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="7.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,6 +638,9 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validar cabeceras del formato de carga de actividades
</commit_message>
<xml_diff>
--- a/media/forma_carga_actividad_plantilla.xlsx
+++ b/media/forma_carga_actividad_plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sersocial-my.sharepoint.com/personal/jrueda_sersocial_org/Documents/Documentos/Proyectos SerSocial/zagilad/zagilad/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E1CD3DF-AC93-4B73-8F27-9D1F79EA47FA}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28D1671E-BE2F-434D-ABE8-949B99930E9E}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,37 +178,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Tipo de Identificación del Usuario</t>
-  </si>
-  <si>
-    <t>Número de Identificación del Usuario en el Sistema</t>
-  </si>
-  <si>
-    <t>Primer Apellido del usuario</t>
-  </si>
-  <si>
-    <t>Segundo apellido del usuario</t>
-  </si>
-  <si>
-    <t>Primer nombre del usuario</t>
-  </si>
-  <si>
-    <t>Segundo nombre del usuario</t>
-  </si>
-  <si>
-    <t>REGIONAL</t>
-  </si>
-  <si>
-    <t>Fecha de la gestion</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>CIE10</t>
-  </si>
-  <si>
-    <t>Identificación médico</t>
+    <t>tipo_identificacion</t>
+  </si>
+  <si>
+    <t>numero_identificacion</t>
+  </si>
+  <si>
+    <t>primer_apellido</t>
+  </si>
+  <si>
+    <t>segundo_apellido</t>
+  </si>
+  <si>
+    <t>primer_nombre</t>
+  </si>
+  <si>
+    <t>segundo_nombre</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>fecha_gestion</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>ciex</t>
+  </si>
+  <si>
+    <t>medico_id</t>
   </si>
 </sst>
 </file>
@@ -322,6 +322,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,7 +594,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,7 +612,7 @@
     <col min="11" max="11" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add Finalidad model and integrate into existing functionality; update admin, views, and migrations for improved activity processing
</commit_message>
<xml_diff>
--- a/media/forma_carga_actividad_plantilla.xlsx
+++ b/media/forma_carga_actividad_plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sersocial-my.sharepoint.com/personal/jrueda_sersocial_org/Documents/Documentos/Proyectos SerSocial/zagilad/zagilad/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28D1671E-BE2F-434D-ABE8-949B99930E9E}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_AD4D2F04E46CFB4ACB3E20FC3D53E176693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{959B1143-3571-4E46-B160-1F0582CB15B7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>tipo_identificacion</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>medico_id</t>
+  </si>
+  <si>
+    <t>finalidad</t>
   </si>
 </sst>
 </file>
@@ -322,10 +325,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +611,7 @@
     <col min="11" max="11" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,6 +644,9 @@
       </c>
       <c r="K1" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>